<commit_message>
fix: correct plot axis order in transactions timeline visualization
</commit_message>
<xml_diff>
--- a/Python/pandas/cajero/transacciones.xlsx
+++ b/Python/pandas/cajero/transacciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,48 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-03-08 12:32:14</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>74887540</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>deposito</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-03-08 12:34:31</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>74887540</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>retiro</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: update binary files for clientes and transacciones spreadsheets
</commit_message>
<xml_diff>
--- a/Python/pandas/cajero/transacciones.xlsx
+++ b/Python/pandas/cajero/transacciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -833,6 +833,27 @@
         <v>100</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-03-08 14:47:17</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>74887540</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>retiro</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>